<commit_message>
popunjene sve xls tablice
</commit_message>
<xml_diff>
--- a/projekt_hoteli.xlsx
+++ b/projekt_hoteli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Desktop\rp2_projekt\rp2_projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95377A4B-8BE1-40A4-8471-5EA6C34B7AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816AB34B-5FAD-41BE-88B9-F6CC48EA3374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="270" windowWidth="6580" windowHeight="9130" firstSheet="3" activeTab="3" xr2:uid="{0F003305-FBA4-4A23-95FC-F5EDBADD91DA}"/>
+    <workbookView xWindow="5800" yWindow="0" windowWidth="6910" windowHeight="10200" firstSheet="2" activeTab="2" xr2:uid="{0F003305-FBA4-4A23-95FC-F5EDBADD91DA}"/>
   </bookViews>
   <sheets>
     <sheet name="hoteli" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>ime</t>
   </si>
@@ -106,12 +106,6 @@
     <t>Anita</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Razmislite o tome da sobu i namještaj i njoj prilagodite i onim gostima koji moraju dulje sjediti za računalom. Stolci u sobi namijenjeni su odmoru i ne dopuštaju dulji rad.</t>
-  </si>
-  <si>
     <t>Dominik</t>
   </si>
   <si>
@@ -139,12 +133,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Izvanredan doručak.</t>
-  </si>
-  <si>
     <t>Hotel Sheraton je uvijek naš odabir kada dolazimo Zagreb. Na odličnoj je lokaciji sa vlastitim parkingom (što je najbitnije ako dolazite vlastitim autom).</t>
   </si>
   <si>
@@ -157,30 +145,12 @@
     <t>Buka od tramvaja s obzirom da s jedne strane hotela prolazi tramvaj cijelo vrijeme boravka je bila prisutna buka.</t>
   </si>
   <si>
-    <t>Nije nam se svidjela jedino kada u sobi. Sve je jednostavno dobro.</t>
-  </si>
-  <si>
-    <t>Isic</t>
-  </si>
-  <si>
     <t>Matko</t>
   </si>
   <si>
     <t>Svidjeli su mi se bazen i sauna.</t>
   </si>
   <si>
-    <t>Galić</t>
-  </si>
-  <si>
-    <t>Dobra lokacija i doručak.</t>
-  </si>
-  <si>
-    <t>Irena</t>
-  </si>
-  <si>
-    <t>Lokacija odlična.Doručak dobar.Osoblje ljubazno.</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
@@ -217,66 +187,24 @@
     <t>Smrad u sobi i namjestaju, te smrad rucnika</t>
   </si>
   <si>
-    <t>Graham</t>
-  </si>
-  <si>
-    <t>Excellent location, beautifully renovated 18th century building in the heart of the old Town. Nothing not to like.</t>
-  </si>
-  <si>
-    <t>Matea</t>
-  </si>
-  <si>
-    <t>Osoblje komunikativno i susretljivo, omogućili su nam raniji ulazak u sobu. Doručak je raznovrstan i ukusan. Lokacija samog hotela, na trgu pored palače, je idealna s obzirom na blizinu svega.</t>
-  </si>
-  <si>
-    <t>Damir</t>
-  </si>
-  <si>
-    <t>Sve pohvale i komplimenti</t>
-  </si>
-  <si>
     <t>Beth</t>
   </si>
   <si>
     <t xml:space="preserve"> The location can’t be better. Close to restaurants and sites.</t>
   </si>
   <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Heritage building well renovated in the center of the old town. we had a great view of the square. Felt like we were in a heritage building, but all the amenities were modern. Close to cafes and waterfront - great room for people watching in the square below you! room was quiet when windows closed.</t>
-  </si>
-  <si>
-    <t>location, cleanliness,room size and friendly staff</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
     <t>Oleh</t>
   </si>
   <si>
     <t> It was awesome hotel and stay; view from room was really stunning; would recommend everyone to stay; will visit again; man on reception when we came was very polite and professional and nice</t>
   </si>
   <si>
-    <t>Jofo1</t>
-  </si>
-  <si>
-    <t>Superb</t>
-  </si>
-  <si>
     <t>Francoise</t>
   </si>
   <si>
     <t>Great view, very clean room, very friendly staff. I was positively surprised by the quality and variety of local products offered for breakfast. Excellent!</t>
   </si>
   <si>
-    <t>Very hot room that was difficult to air and cool</t>
-  </si>
-  <si>
-    <t>Jelenahaj</t>
-  </si>
-  <si>
     <t>Irina</t>
   </si>
   <si>
@@ -322,27 +250,9 @@
     <t>Stephen</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Food and service were exceptional</t>
-  </si>
-  <si>
     <t>Spacious room w balcony.</t>
   </si>
   <si>
-    <t>Nice quiet location. Not far from center</t>
-  </si>
-  <si>
-    <t>The hotel is very easy to find. The property has its own small car park... please avoid parking with large cars. The living room table has enough space for a laptop. Breakfast is from 7 am...nothing special, but you can find something for yourself.</t>
-  </si>
-  <si>
-    <t>Dean</t>
-  </si>
-  <si>
-    <t>Dubravko</t>
-  </si>
-  <si>
     <t>I am a bit of a picky person but the staff, facilities and breakfast was all great. Staff was very friendly and made us feel very welcome</t>
   </si>
   <si>
@@ -355,24 +265,12 @@
     <t>Pool was closed and door sound isolation could be better</t>
   </si>
   <si>
-    <t>Branka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Music during breakfast wasn’t my taste. Room was too hot because of underfloor heating but this was adjusted. Need a magnifying mirror in the bathroom for the ladies applying their makeup </t>
-  </si>
-  <si>
-    <t>Rene</t>
-  </si>
-  <si>
     <t>Slavisa</t>
   </si>
   <si>
     <t>Hermina</t>
   </si>
   <si>
-    <t>the best breakfast and very good service ! we will come again !</t>
-  </si>
-  <si>
     <t>Excellent breakfast, great selection. Clean and tidy hotel, great location</t>
   </si>
   <si>
@@ -385,39 +283,9 @@
     <t>good location for our purpose. it is a bit old but good overall. doesn’t have a lift so a bit of a trek to go upstairs with luggage or heavy bags</t>
   </si>
   <si>
-    <t>Carly</t>
-  </si>
-  <si>
-    <t>EVERYTHING! we enjoyed the most wonderful stay! peaceful, relaxing, calming, wonderful owner and staff who cannot do enough for you, superb home cooked and baked food, stunning comfortable and well equipped room, beautiful grounds. we were so well looked after. they have thought of everything! superb!</t>
-  </si>
-  <si>
-    <t>Hitch6666</t>
-  </si>
-  <si>
-    <t>Breakfast was awesome, and hospitality. Bed bugs in one of our rooms</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t> Everything was magnificent. The room cleanliness, the cute decor, the fresh, homemade breakfasts in the garden every morning, the sweet staff members and owner made us wish we could stay longer.</t>
-  </si>
-  <si>
-    <t>Christi</t>
-  </si>
-  <si>
-    <t>What a pleasant surprise really more of a B&amp;B than just a room for rent. The staff was incredibly helpful and informative. Breakfast was absolutely delicious.</t>
-  </si>
-  <si>
-    <t>Jenny</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
-    <t>Everything, but most of all the staff🎈extraordinary.</t>
-  </si>
-  <si>
     <t>Rooms were small but modern appliances. Staff outstanding. 3 course lamb dinner very good. Large parking in back. Only 4 lounge chairs at pool</t>
   </si>
   <si>
@@ -433,12 +301,6 @@
     <t>Great location and check in staff member was very helpful. The breakfast was amazing.  We weren’t told that the pool was empty.</t>
   </si>
   <si>
-    <t>Eleonora</t>
-  </si>
-  <si>
-    <t>Perfect place if you want get some rest, close to few beaches restaurants and bars supermarket just 2 minute walk from the hotel. Amazing breakfast lots of choices, very nice and kind stuff, the room was clean with a lovely balcony. If you want to go to the old town is 40/50 min walk or you can get a bus, but the public transport are not great at all.</t>
-  </si>
-  <si>
     <t>Debra</t>
   </si>
   <si>
@@ -518,6 +380,81 @@
   </si>
   <si>
     <t>Studio with Balcony</t>
+  </si>
+  <si>
+    <t>6.8.2023.</t>
+  </si>
+  <si>
+    <t>9.8.2023.</t>
+  </si>
+  <si>
+    <t>10.8.2023.</t>
+  </si>
+  <si>
+    <t>30.8.2023.</t>
+  </si>
+  <si>
+    <t>20.8.2023.</t>
+  </si>
+  <si>
+    <t>15.7.2023.</t>
+  </si>
+  <si>
+    <t>11.8.2023.</t>
+  </si>
+  <si>
+    <t>16.9.2023.</t>
+  </si>
+  <si>
+    <t>25.8.2023.</t>
+  </si>
+  <si>
+    <t>10.12.2023.</t>
+  </si>
+  <si>
+    <t>1.10.2023.</t>
+  </si>
+  <si>
+    <t>2.11.2023.</t>
+  </si>
+  <si>
+    <t>5.8.2023</t>
+  </si>
+  <si>
+    <t>19.8.2023.</t>
+  </si>
+  <si>
+    <t>27.7.2023</t>
+  </si>
+  <si>
+    <t>8.8.2023.</t>
+  </si>
+  <si>
+    <t>28.7.2023.</t>
+  </si>
+  <si>
+    <t>18.7.2023</t>
+  </si>
+  <si>
+    <t>19.7.2023.</t>
+  </si>
+  <si>
+    <t>26.7.2023</t>
+  </si>
+  <si>
+    <t>31.7.2023.</t>
+  </si>
+  <si>
+    <t>16.8.2023</t>
+  </si>
+  <si>
+    <t>31.8.2023.</t>
+  </si>
+  <si>
+    <t>24.8.2023</t>
+  </si>
+  <si>
+    <t>4.9.2023.</t>
   </si>
 </sst>
 </file>
@@ -562,9 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,7 +954,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="B9">
         <v>13</v>
@@ -1105,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1223,15 +1161,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AB1441-C471-46DD-A014-CF2062584065}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1242,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -1273,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1282,32 +1220,32 @@
         <v>26</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
@@ -1316,21 +1254,21 @@
         <v>37</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1338,10 +1276,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -1355,27 +1293,27 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
       <c r="E8">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -1389,10 +1327,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
@@ -1401,15 +1339,15 @@
         <v>47</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
@@ -1423,10 +1361,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
@@ -1435,15 +1373,15 @@
         <v>51</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
@@ -1452,15 +1390,15 @@
         <v>53</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -1474,10 +1412,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>56</v>
@@ -1486,15 +1424,15 @@
         <v>57</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>58</v>
@@ -1508,10 +1446,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -1520,15 +1458,15 @@
         <v>61</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>62</v>
@@ -1542,10 +1480,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>64</v>
@@ -1559,10 +1497,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>66</v>
@@ -1571,15 +1509,15 @@
         <v>67</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
@@ -1588,15 +1526,15 @@
         <v>69</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
@@ -1610,33 +1548,33 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
       <c r="E23">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
         <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>75</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1644,10 +1582,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
@@ -1661,33 +1599,33 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
         <v>81</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
       </c>
       <c r="E27">
         <v>8</v>
@@ -1695,10 +1633,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
         <v>82</v>
@@ -1707,15 +1645,15 @@
         <v>83</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
         <v>84</v>
@@ -1724,15 +1662,15 @@
         <v>85</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>86</v>
@@ -1746,44 +1684,44 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B32">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B33">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
         <v>92</v>
@@ -1792,397 +1730,6 @@
         <v>93</v>
       </c>
       <c r="E33">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>11</v>
-      </c>
-      <c r="B34">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>16</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>17</v>
-      </c>
-      <c r="B36">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>17</v>
-      </c>
-      <c r="B37">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>17</v>
-      </c>
-      <c r="B38">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>17</v>
-      </c>
-      <c r="B39">
-        <v>39</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>17</v>
-      </c>
-      <c r="B40">
-        <v>40</v>
-      </c>
-      <c r="C40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>16</v>
-      </c>
-      <c r="B41">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" t="s">
-        <v>109</v>
-      </c>
-      <c r="E41">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>16</v>
-      </c>
-      <c r="B42">
-        <v>42</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" t="s">
-        <v>113</v>
-      </c>
-      <c r="E42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>16</v>
-      </c>
-      <c r="B43">
-        <v>43</v>
-      </c>
-      <c r="C43" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>16</v>
-      </c>
-      <c r="B44">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" t="s">
-        <v>115</v>
-      </c>
-      <c r="E44">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>16</v>
-      </c>
-      <c r="B45">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" t="s">
-        <v>117</v>
-      </c>
-      <c r="E45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>21</v>
-      </c>
-      <c r="B46">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" t="s">
-        <v>119</v>
-      </c>
-      <c r="E46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>21</v>
-      </c>
-      <c r="B47">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" t="s">
-        <v>121</v>
-      </c>
-      <c r="E47">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>22</v>
-      </c>
-      <c r="B48">
-        <v>48</v>
-      </c>
-      <c r="C48" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" t="s">
-        <v>123</v>
-      </c>
-      <c r="E48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>22</v>
-      </c>
-      <c r="B49">
-        <v>49</v>
-      </c>
-      <c r="C49" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" t="s">
-        <v>125</v>
-      </c>
-      <c r="E49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>22</v>
-      </c>
-      <c r="B50">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>22</v>
-      </c>
-      <c r="B51">
-        <v>51</v>
-      </c>
-      <c r="C51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D51" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>22</v>
-      </c>
-      <c r="B52">
-        <v>52</v>
-      </c>
-      <c r="C52" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" t="s">
-        <v>131</v>
-      </c>
-      <c r="E52">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>21</v>
-      </c>
-      <c r="B53">
-        <v>53</v>
-      </c>
-      <c r="C53" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>21</v>
-      </c>
-      <c r="B54">
-        <v>54</v>
-      </c>
-      <c r="C54" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" t="s">
-        <v>137</v>
-      </c>
-      <c r="E54">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>21</v>
-      </c>
-      <c r="B55">
-        <v>55</v>
-      </c>
-      <c r="C55" t="s">
-        <v>132</v>
-      </c>
-      <c r="D55" t="s">
-        <v>133</v>
-      </c>
-      <c r="E55">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>21</v>
-      </c>
-      <c r="B56">
-        <v>56</v>
-      </c>
-      <c r="C56" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56">
         <v>8</v>
       </c>
     </row>
@@ -2197,543 +1744,279 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE612EE-B4AC-42D9-83B6-0503EF81A43E}">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="2">
+        <v>45146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>55</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45199</v>
+      </c>
+      <c r="C12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45231</v>
+      </c>
+      <c r="C13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>14</v>
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45154</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A102">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A103">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A104">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A105">
-        <v>104</v>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2745,24 +2028,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF15C255-F5FA-4601-82AC-36E4FD56FA66}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2776,7 +2059,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2790,7 +2073,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2804,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2818,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2832,7 +2115,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2846,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2860,7 +2143,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2874,7 +2157,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -2888,7 +2171,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2902,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2916,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2930,7 +2213,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -2944,7 +2227,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -2958,7 +2241,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -2972,7 +2255,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -2986,7 +2269,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -3000,7 +2283,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -3014,7 +2297,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -3028,7 +2311,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -3042,7 +2325,7 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -3056,7 +2339,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -3070,7 +2353,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -3084,7 +2367,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -3098,7 +2381,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -3112,7 +2395,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -3126,7 +2409,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -3140,7 +2423,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -3154,7 +2437,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -3168,7 +2451,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -3182,7 +2465,7 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -3196,7 +2479,7 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -3210,7 +2493,7 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -3224,7 +2507,7 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -3238,7 +2521,7 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -3252,7 +2535,7 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -3266,7 +2549,7 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -3280,7 +2563,7 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -3294,7 +2577,7 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -3308,7 +2591,7 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -3322,7 +2605,7 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -3336,7 +2619,7 @@
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -3350,7 +2633,7 @@
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -3364,7 +2647,7 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -3378,7 +2661,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -3392,7 +2675,7 @@
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -3406,7 +2689,7 @@
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -3420,7 +2703,7 @@
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -3434,7 +2717,7 @@
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -3448,7 +2731,7 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -3462,7 +2745,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -3476,7 +2759,7 @@
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -3490,7 +2773,7 @@
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -3504,7 +2787,7 @@
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -3518,7 +2801,7 @@
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -3532,7 +2815,7 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -3546,7 +2829,7 @@
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -3560,7 +2843,7 @@
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -3574,7 +2857,7 @@
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -3588,7 +2871,7 @@
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -3602,7 +2885,7 @@
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -3616,7 +2899,7 @@
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -3630,7 +2913,7 @@
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -3644,7 +2927,7 @@
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -3652,13 +2935,13 @@
         <v>72</v>
       </c>
       <c r="B65">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C65">
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -3672,7 +2955,7 @@
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -3686,7 +2969,7 @@
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -3700,7 +2983,7 @@
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -3714,7 +2997,7 @@
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -3728,7 +3011,7 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -3742,7 +3025,7 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -3756,7 +3039,7 @@
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -3770,7 +3053,7 @@
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -3784,7 +3067,7 @@
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -3798,7 +3081,7 @@
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
@@ -3812,7 +3095,7 @@
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -3826,7 +3109,7 @@
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -3840,7 +3123,7 @@
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -3854,7 +3137,7 @@
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -3868,7 +3151,7 @@
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -3882,7 +3165,7 @@
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -3890,13 +3173,13 @@
         <v>72</v>
       </c>
       <c r="B82">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -3910,7 +3193,7 @@
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
@@ -3924,7 +3207,7 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -3938,7 +3221,7 @@
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
@@ -3952,7 +3235,7 @@
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
@@ -3966,7 +3249,7 @@
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
@@ -3980,7 +3263,7 @@
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -3994,7 +3277,7 @@
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -4008,7 +3291,7 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -4022,7 +3305,7 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -4036,7 +3319,7 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
@@ -4050,7 +3333,7 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
@@ -4064,7 +3347,7 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
@@ -4078,7 +3361,7 @@
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
@@ -4092,7 +3375,7 @@
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -4106,7 +3389,7 @@
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
@@ -4120,7 +3403,7 @@
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -4134,7 +3417,7 @@
         <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -4148,7 +3431,7 @@
         <v>99</v>
       </c>
       <c r="D100" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
@@ -4156,13 +3439,13 @@
         <v>72</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C101">
         <v>100</v>
       </c>
       <c r="D101" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
@@ -4176,7 +3459,7 @@
         <v>101</v>
       </c>
       <c r="D102" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
@@ -4190,7 +3473,7 @@
         <v>102</v>
       </c>
       <c r="D103" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -4204,7 +3487,7 @@
         <v>103</v>
       </c>
       <c r="D104" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -4218,7 +3501,7 @@
         <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>